<commit_message>
haiph1210- update file and client.
</commit_message>
<xml_diff>
--- a/ExcelFile/fileChamCong.xlsx
+++ b/ExcelFile/fileChamCong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MRS_YangkangRestaurant\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5A1EFA-93E0-4C60-B076-0E2EEDB5E271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB33581A-C1A1-4537-BEC0-8ED804FAC5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B302FD84-A00F-4439-AB89-5E3883574C06}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Mã Nhân Viên</t>
   </si>
@@ -51,18 +51,6 @@
     <t>Nửa Ngày</t>
   </si>
   <si>
-    <t>HAIPH-1</t>
-  </si>
-  <si>
-    <t>TRANGTR-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Không </t>
-  </si>
-  <si>
-    <t>Có</t>
-  </si>
-  <si>
     <t>Cả Ngày</t>
   </si>
   <si>
@@ -70,6 +58,21 @@
   </si>
   <si>
     <t>Ngày</t>
+  </si>
+  <si>
+    <t>QUANGHAI</t>
+  </si>
+  <si>
+    <t>Quản Lí</t>
+  </si>
+  <si>
+    <t>HAIPHAM</t>
+  </si>
+  <si>
+    <t>Quang Hải Chấm Công</t>
+  </si>
+  <si>
+    <t>Phạm Hải Chấm Công</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBD0C04-DA82-4855-8C96-63C98FADC41D}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -457,6 +462,7 @@
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -464,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -478,36 +484,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>45082</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>45082</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>